<commit_message>
Issue with Compiling common code
</commit_message>
<xml_diff>
--- a/src/aot/NativeAOT.xlsx
+++ b/src/aot/NativeAOT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Core\LakshanF\CSharp\src\aot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E346F4DA-F2A0-406C-84CD-F5D376121128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70290A6-FA78-40B9-8C3E-23A463EA02EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="SDK" sheetId="4" r:id="rId1"/>
@@ -22,8 +22,9 @@
     <sheet name="CMake" sheetId="8" r:id="rId7"/>
     <sheet name="Port" sheetId="9" r:id="rId8"/>
     <sheet name="Port_Issues" sheetId="10" r:id="rId9"/>
-    <sheet name="ds_server_init" sheetId="11" r:id="rId10"/>
-    <sheet name="scratch" sheetId="5" r:id="rId11"/>
+    <sheet name="Port-Tables" sheetId="12" r:id="rId10"/>
+    <sheet name="ds_server_init" sheetId="11" r:id="rId11"/>
+    <sheet name="scratch" sheetId="5" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="417">
   <si>
     <t>File</t>
   </si>
@@ -1475,9 +1476,6 @@
     <t>Can't find header files</t>
   </si>
   <si>
-    <t>Aaron helped with finding the root dir for build (artifacts/bin/coreclr/windows.x64.Release) + cheat by including the INCLUDE file</t>
-  </si>
-  <si>
     <t>Issue</t>
   </si>
   <si>
@@ -1679,6 +1677,147 @@
   </si>
   <si>
     <t>ep_rt_val_int16_t</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>_rt_coreclr_table_callbacks_t</t>
+  </si>
+  <si>
+    <t>(*key_free_func)(void *)</t>
+  </si>
+  <si>
+    <t>(*value_free_func)(void *)</t>
+  </si>
+  <si>
+    <t>SHash&lt;NoRemoveSHashTraits&lt; MapSHashTraits &lt;T1, T2&gt; &gt; &gt; table_type_t;</t>
+  </si>
+  <si>
+    <t>MapSHashTraits&lt;K,V&gt;</t>
+  </si>
+  <si>
+    <t>DefaultSHashTraits&lt;Element&gt;</t>
+  </si>
+  <si>
+    <t>KeyValuePair&lt;K,V&gt;</t>
+  </si>
+  <si>
+    <t>DefaultSHashTraits&lt;KVP&lt;K,V&gt;&gt;</t>
+  </si>
+  <si>
+    <t>NoRemoveSHashTraits&lt;Parent&gt;</t>
+  </si>
+  <si>
+    <t>Parent:element_t</t>
+  </si>
+  <si>
+    <t>Parent:count_t</t>
+  </si>
+  <si>
+    <t>DefaultSHashTraits:element_t</t>
+  </si>
+  <si>
+    <t>DefaultSHashTraits:count_t</t>
+  </si>
+  <si>
+    <t>UINT32:count_t</t>
+  </si>
+  <si>
+    <t>ELEMENT:element_t</t>
+  </si>
+  <si>
+    <t>Shash&lt;Traits&gt;</t>
+  </si>
+  <si>
+    <t>TRAITS::element_t element_t</t>
+  </si>
+  <si>
+    <t>TRAITS::PTR_element_t PTR_element_t</t>
+  </si>
+  <si>
+    <t>noncopyable</t>
+  </si>
+  <si>
+    <t>TRAITS::key_t key_t</t>
+  </si>
+  <si>
+    <t>TRAITS::count_t count_t</t>
+  </si>
+  <si>
+    <t>_rt_coreclr_table_default_internal_t&lt;T1, T2&gt;</t>
+  </si>
+  <si>
+    <t>_rt_coreclr_table_remove_internal_t&lt;T1, T2&gt;</t>
+  </si>
+  <si>
+    <t>rt_coreclr_table_callbacks_t callbacks;</t>
+  </si>
+  <si>
+    <t>EventPipeCoreCLRStackHashTraits</t>
+  </si>
+  <si>
+    <t>Extends public NoRemoveSHashTraits&lt; MapSHashTraits&lt;StackHashKey *, StackHashEntry *&gt; &gt;</t>
+  </si>
+  <si>
+    <t>MapSHashTraits&lt;StackHashKey *, StackHashEntry *&gt;::element_t element_t;</t>
+  </si>
+  <si>
+    <t>MapSHashTraits&lt;StackHashKey *, StackHashEntry *&gt;::count_t count_t;</t>
+  </si>
+  <si>
+    <t>_rt_coreclr_table_custom_internal_t&lt;T&gt;</t>
+  </si>
+  <si>
+    <t>SHash&lt;T1&gt; table_type_t;</t>
+  </si>
+  <si>
+    <t>table_type_t *table;</t>
+  </si>
+  <si>
+    <t>_rt_coreclr_event_internal_t</t>
+  </si>
+  <si>
+    <t>CLREventStatic *event;</t>
+  </si>
+  <si>
+    <t>_rt_coreclr_lock_internal_t</t>
+  </si>
+  <si>
+    <t>CrstStatic *lock;</t>
+  </si>
+  <si>
+    <t>_rt_coreclr_spin_lock_internal_t</t>
+  </si>
+  <si>
+    <t>SpinLock *lock;</t>
+  </si>
+  <si>
+    <t>Collection Type</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>EmptyContainer.h</t>
+  </si>
+  <si>
+    <t>Not all public properties</t>
+  </si>
+  <si>
+    <t>Aaron helped with finding the root dir for build (artifacts\obj\coreclr\windows.x64.Release) + cheat by including the INCLUDE file (dev command line)</t>
+  </si>
+  <si>
+    <t>step6</t>
+  </si>
+  <si>
+    <t>Compile Common code</t>
+  </si>
+  <si>
+    <t>Common code knows how to pick aot shim files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issue with compiling </t>
   </si>
 </sst>
 </file>
@@ -2162,7 +2301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BA1F5E-206C-47BA-9ABB-2AD1328C0FAB}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2346,6 +2485,209 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D2F1AD-2A04-472D-8139-884175DD7E01}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E1" t="s">
+        <v>409</v>
+      </c>
+      <c r="F1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>376</v>
+      </c>
+      <c r="F4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B5" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>393</v>
+      </c>
+      <c r="B8" t="s">
+        <v>374</v>
+      </c>
+      <c r="D8" t="s">
+        <v>375</v>
+      </c>
+      <c r="E8" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>394</v>
+      </c>
+      <c r="D9" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>395</v>
+      </c>
+      <c r="B11" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>397</v>
+      </c>
+      <c r="D12" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>398</v>
+      </c>
+      <c r="D13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>399</v>
+      </c>
+      <c r="B15" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>394</v>
+      </c>
+      <c r="D16" t="s">
+        <v>386</v>
+      </c>
+      <c r="E16" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>401</v>
+      </c>
+      <c r="D17" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>402</v>
+      </c>
+      <c r="B19" t="s">
+        <v>403</v>
+      </c>
+      <c r="D19" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>404</v>
+      </c>
+      <c r="B21" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>406</v>
+      </c>
+      <c r="B23" t="s">
+        <v>407</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5CE37D-047E-48E6-B103-516D9C44DD99}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2368,35 +2710,35 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B3" t="s">
         <v>346</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>347</v>
-      </c>
-      <c r="D3" t="s">
-        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -2404,7 +2746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E79789-F7A8-4F49-8B82-CFB73A3CAE8C}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -3568,10 +3910,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA29BBC-4F7B-49AE-9AF5-58895851EE5E}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3650,7 +3992,7 @@
         <v>260</v>
       </c>
       <c r="E4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3709,7 +4051,7 @@
         <v>279</v>
       </c>
       <c r="B8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C8" t="s">
         <v>273</v>
@@ -3842,7 +4184,7 @@
         <v>297</v>
       </c>
       <c r="B16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C16" t="s">
         <v>294</v>
@@ -3854,7 +4196,7 @@
         <v>308</v>
       </c>
       <c r="F16" t="s">
-        <v>309</v>
+        <v>412</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3862,19 +4204,19 @@
         <v>297</v>
       </c>
       <c r="B17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C17" t="s">
         <v>294</v>
       </c>
       <c r="D17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E17" t="s">
+        <v>335</v>
+      </c>
+      <c r="F17" t="s">
         <v>336</v>
-      </c>
-      <c r="F17" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3882,64 +4224,78 @@
         <v>297</v>
       </c>
       <c r="B18" t="s">
+        <v>337</v>
+      </c>
+      <c r="C18" t="s">
         <v>338</v>
       </c>
-      <c r="C18" t="s">
-        <v>339</v>
-      </c>
       <c r="D18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B19" t="s">
+        <v>359</v>
+      </c>
+      <c r="C19" t="s">
         <v>360</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>361</v>
-      </c>
-      <c r="D19" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B20" t="s">
+        <v>359</v>
+      </c>
+      <c r="C20" t="s">
         <v>360</v>
       </c>
-      <c r="C20" t="s">
-        <v>361</v>
-      </c>
       <c r="D20" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B21" t="s">
+        <v>366</v>
+      </c>
+      <c r="C21" t="s">
         <v>367</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>368</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>370</v>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>413</v>
+      </c>
+      <c r="B22" t="s">
+        <v>414</v>
+      </c>
+      <c r="C22" t="s">
+        <v>415</v>
+      </c>
+      <c r="D22" t="s">
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -3954,7 +4310,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3967,19 +4323,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D1" t="s">
         <v>310</v>
       </c>
-      <c r="D1" t="s">
-        <v>311</v>
-      </c>
       <c r="E1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -3987,13 +4343,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D2" t="s">
         <v>312</v>
       </c>
-      <c r="D2" t="s">
-        <v>313</v>
-      </c>
       <c r="E2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F2" t="s">
         <v>284</v>
@@ -4004,52 +4360,52 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E3" t="s">
         <v>316</v>
       </c>
-      <c r="E3" t="s">
-        <v>317</v>
-      </c>
       <c r="F3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
+        <v>317</v>
+      </c>
+      <c r="D4" t="s">
         <v>318</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>319</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>320</v>
-      </c>
-      <c r="F4" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>322</v>
+      </c>
+      <c r="D5" t="s">
         <v>323</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>324</v>
-      </c>
-      <c r="E5" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>329</v>
+      </c>
+      <c r="D6" t="s">
         <v>330</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>331</v>
-      </c>
-      <c r="E6" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4057,10 +4413,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4068,16 +4424,16 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
+        <v>355</v>
+      </c>
+      <c r="C8" t="s">
+        <v>351</v>
+      </c>
+      <c r="D8" t="s">
         <v>356</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>352</v>
-      </c>
-      <c r="D8" t="s">
-        <v>357</v>
-      </c>
-      <c r="E8" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4085,31 +4441,31 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D9" t="s">
+        <v>364</v>
+      </c>
+      <c r="E9" t="s">
         <v>365</v>
-      </c>
-      <c r="E9" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
current checkpoint with empty container and runtime but startup failing with hooks
</commit_message>
<xml_diff>
--- a/src/aot/NativeAOT.xlsx
+++ b/src/aot/NativeAOT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Core\LakshanF\CSharp\src\aot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70290A6-FA78-40B9-8C3E-23A463EA02EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44A5C3C-F52F-43DC-B439-241679D6FB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
   </bookViews>
@@ -27,7 +27,6 @@
     <sheet name="scratch" sheetId="5" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="436">
   <si>
     <t>File</t>
   </si>
@@ -1817,7 +1816,64 @@
     <t>Common code knows how to pick aot shim files</t>
   </si>
   <si>
-    <t xml:space="preserve">Issue with compiling </t>
+    <t xml:space="preserve">'-IC:\Work\Core\CurrentWork\runtime\artifacts\obj\coreclr\windows.x64.Release\nativeaot\Runtime\Full </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'-IC:\Work\Core\CurrentWork\runtime\src\coreclr\nativeaot\Runtime\Full </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'-IC:\Work\Core\CurrentWork\runtime\src\native </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'-IC:\Work\Core\CurrentWork\runtime\src\coreclr\pal\prebuilt\inc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'-IC:\Work\Core\CurrentWork\runtime\artifacts\obj </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'-IC:\Work\Core\CurrentWork\runtime\src\native\eventpipe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'-IC:\Work\Core\CurrentWork\runtime\src\coreclr\nativeaot\Runtime\inc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'-IC:\Work\Core\CurrentWork\runtime\src\coreclr\nativeaot\Runtime\. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'-IC:\Work\Core\CurrentWork\runtime\src\coreclr\nativeaot\Runtime\..\..\gc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'-IC:\Work\Core\CurrentWork\runtime\src\coreclr\nativeaot\Runtime\..\..\gc\env </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'-IC:\Work\Core\CurrentWork\runtime\src\coreclr\nativeaot\Runtime\windows </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'-IC:\Work\Core\CurrentWork\runtime\src\coreclr\nativeaot\Runtime\amd64 </t>
+  </si>
+  <si>
+    <t>step7</t>
+  </si>
+  <si>
+    <t>Issue with compiling common header files</t>
+  </si>
+  <si>
+    <t>Don’t compile common header files as C++ (/TP)</t>
+  </si>
+  <si>
+    <t>Compile DS (Diagnostic Server code)</t>
+  </si>
+  <si>
+    <t>Error free for DS server</t>
+  </si>
+  <si>
+    <t>LF_DIAGNOSTICS_PORT</t>
+  </si>
+  <si>
+    <t>This is cause common code calls functions like DS_LOG_ERROR_2, which in coreclr has the constant defined</t>
+  </si>
+  <si>
+    <t>Tried getting to these constants via stressLog.h but trying to punt for now</t>
   </si>
 </sst>
 </file>
@@ -2489,7 +2545,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3910,10 +3966,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA29BBC-4F7B-49AE-9AF5-58895851EE5E}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3921,7 +3977,7 @@
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="82.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="97.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4295,7 +4351,30 @@
         <v>415</v>
       </c>
       <c r="D22" t="s">
-        <v>416</v>
+        <v>429</v>
+      </c>
+      <c r="E22" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>428</v>
+      </c>
+      <c r="B23" t="s">
+        <v>431</v>
+      </c>
+      <c r="C23" t="s">
+        <v>432</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="E23" t="s">
+        <v>434</v>
+      </c>
+      <c r="F23" t="s">
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -4307,17 +4386,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8B967F-830C-4BFE-AD9E-62679C946E39}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="83.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="99.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4466,6 +4545,66 @@
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>334</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
current status of port helper artifacts
</commit_message>
<xml_diff>
--- a/src/aot/NativeAOT.xlsx
+++ b/src/aot/NativeAOT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Core\LakshanF\CSharp\src\aot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44A5C3C-F52F-43DC-B439-241679D6FB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4BE3B4-859C-4C31-B204-8F0E9213D2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="12" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="SDK" sheetId="4" r:id="rId1"/>
@@ -21,10 +21,11 @@
     <sheet name="clr.aot" sheetId="7" r:id="rId6"/>
     <sheet name="CMake" sheetId="8" r:id="rId7"/>
     <sheet name="Port" sheetId="9" r:id="rId8"/>
-    <sheet name="Port_Issues" sheetId="10" r:id="rId9"/>
-    <sheet name="Port-Tables" sheetId="12" r:id="rId10"/>
-    <sheet name="ds_server_init" sheetId="11" r:id="rId11"/>
-    <sheet name="scratch" sheetId="5" r:id="rId12"/>
+    <sheet name="Port_Issues-compiler" sheetId="10" r:id="rId9"/>
+    <sheet name="Port-Issues-linker" sheetId="13" r:id="rId10"/>
+    <sheet name="Port-Tables" sheetId="12" r:id="rId11"/>
+    <sheet name="EP_Init" sheetId="14" r:id="rId12"/>
+    <sheet name="scratch" sheetId="5" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="611">
   <si>
     <t>File</t>
   </si>
@@ -956,36 +957,9 @@
     <t>Details</t>
   </si>
   <si>
-    <t>CrossGen2.csproj</t>
-  </si>
-  <si>
-    <t>ILCompiler.csproj</t>
-  </si>
-  <si>
-    <t>runtime.proj</t>
-  </si>
-  <si>
-    <t>Microsoft.DotNet.ILCompiler.pkgproj</t>
-  </si>
-  <si>
-    <t>Target:BuildRuntime</t>
-  </si>
-  <si>
-    <t>Target:GetILCCompileFiles</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>can be Runtime.ServerGC as well</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>src\coreclr\build-runtime.cmd</t>
-  </si>
-  <si>
     <t>NativeLibrary</t>
   </si>
   <si>
@@ -1184,9 +1158,6 @@
     <t>build and publish experience can be different, the targets in ilc pkgs are the same due to implementation detail</t>
   </si>
   <si>
-    <t>?Full-runtime.*GC.lib</t>
-  </si>
-  <si>
     <t>Artifact</t>
   </si>
   <si>
@@ -1568,22 +1539,10 @@
     <t>ENABLE_PERFTRACING</t>
   </si>
   <si>
-    <t>class</t>
-  </si>
-  <si>
-    <t>DiagnosticServerAdapter</t>
-  </si>
-  <si>
-    <t>API</t>
-  </si>
-  <si>
     <t>ds_server_init</t>
   </si>
   <si>
     <t>ds-server.c</t>
-  </si>
-  <si>
-    <t>Common</t>
   </si>
   <si>
     <t>ds-ipc.c</t>
@@ -1875,12 +1834,579 @@
   <si>
     <t>Tried getting to these constants via stressLog.h but trying to punt for now</t>
   </si>
+  <si>
+    <t>\\chrisahnx74\LakshanF</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>bool __cdecl ds_ipc_pal_init(void)</t>
+  </si>
+  <si>
+    <t>Caller method</t>
+  </si>
+  <si>
+    <t>Caller file</t>
+  </si>
+  <si>
+    <t>Calle file</t>
+  </si>
+  <si>
+    <t>ds-ipc-pal-namedpipe.c</t>
+  </si>
+  <si>
+    <t>ep-block.c</t>
+  </si>
+  <si>
+    <t>ep-buffer-manager.c</t>
+  </si>
+  <si>
+    <t>ep-buffer.c</t>
+  </si>
+  <si>
+    <t>ep-config.c</t>
+  </si>
+  <si>
+    <t>ep-event-instance.c</t>
+  </si>
+  <si>
+    <t>ep-event-payload.c</t>
+  </si>
+  <si>
+    <t>ep-event-source.c</t>
+  </si>
+  <si>
+    <t>ep-event.c</t>
+  </si>
+  <si>
+    <t>ep-file.c</t>
+  </si>
+  <si>
+    <t>ep-json-file.c</t>
+  </si>
+  <si>
+    <t>ep-metadata-generator.c</t>
+  </si>
+  <si>
+    <t>ep-provider.c</t>
+  </si>
+  <si>
+    <t>ep-sample-profiler.c</t>
+  </si>
+  <si>
+    <t>ep-session-provider.c</t>
+  </si>
+  <si>
+    <t>ep-session.c</t>
+  </si>
+  <si>
+    <t>ep-sources.c</t>
+  </si>
+  <si>
+    <t>ep-stack-contents.c</t>
+  </si>
+  <si>
+    <t>ep-stream.c</t>
+  </si>
+  <si>
+    <t>ep-thread.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-sources.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-block.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-buffer.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-buffer-manager.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-config.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-event.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-event-instance.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-event-payload.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-event-source.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-file.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-json-file.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-metadata-generator.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-provider.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-sample-profiler.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-session.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-session-provider.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-stack-contents.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-stream.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ep-thread.c</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>ep*.c</t>
+  </si>
+  <si>
+    <t>ep*.h</t>
+  </si>
+  <si>
+    <t>ds*.c</t>
+  </si>
+  <si>
+    <t>ds*.h</t>
+  </si>
+  <si>
+    <t>configure.cmake</t>
+  </si>
+  <si>
+    <t>CMakeLists.txt</t>
+  </si>
+  <si>
+    <t>README.md</t>
+  </si>
+  <si>
+    <t>ep-shared-config.h.in</t>
+  </si>
+  <si>
+    <t>cmake</t>
+  </si>
+  <si>
+    <t>dir</t>
+  </si>
+  <si>
+    <t>ep.h</t>
+  </si>
+  <si>
+    <t>ep-block.h</t>
+  </si>
+  <si>
+    <t>ep-buffer.h</t>
+  </si>
+  <si>
+    <t>ep-buffer-manager.h</t>
+  </si>
+  <si>
+    <t>ep-config.h</t>
+  </si>
+  <si>
+    <t>ep-config-internals.h</t>
+  </si>
+  <si>
+    <t>ep-event.h</t>
+  </si>
+  <si>
+    <t>ep-event-instance.h</t>
+  </si>
+  <si>
+    <t>ep-event-payload.h</t>
+  </si>
+  <si>
+    <t>ep-event-source.h</t>
+  </si>
+  <si>
+    <t>ep-file.h</t>
+  </si>
+  <si>
+    <t>ep-getter-setter.h</t>
+  </si>
+  <si>
+    <t>ep-ipc-pal-types.h</t>
+  </si>
+  <si>
+    <t>ep-ipc-pal-types-forward.h</t>
+  </si>
+  <si>
+    <t>ep-ipc-stream.h</t>
+  </si>
+  <si>
+    <t>ep-json-file.h</t>
+  </si>
+  <si>
+    <t>ep-metadata-generator.h</t>
+  </si>
+  <si>
+    <t>ep-provider.h</t>
+  </si>
+  <si>
+    <t>ep-provider-internals.h</t>
+  </si>
+  <si>
+    <t>ep-rt.h</t>
+  </si>
+  <si>
+    <t>ep-rt-config.h</t>
+  </si>
+  <si>
+    <t>ep-rt-types.h</t>
+  </si>
+  <si>
+    <t>ep-sample-profiler.h</t>
+  </si>
+  <si>
+    <t>ep-session.h</t>
+  </si>
+  <si>
+    <t>ep-session-provider.h</t>
+  </si>
+  <si>
+    <t>ep-stack-contents.h</t>
+  </si>
+  <si>
+    <t>ep-stream.h</t>
+  </si>
+  <si>
+    <t>ep-thread.h</t>
+  </si>
+  <si>
+    <t>ep-types.h</t>
+  </si>
+  <si>
+    <t>ep-types-forward.h</t>
+  </si>
+  <si>
+    <t>ds-sources.c</t>
+  </si>
+  <si>
+    <t>ds-dump-protocol.c</t>
+  </si>
+  <si>
+    <t>ds-eventpipe-protocol.c</t>
+  </si>
+  <si>
+    <t>ds-process-protocol.c</t>
+  </si>
+  <si>
+    <t>ds-profiler-protocol.c</t>
+  </si>
+  <si>
+    <t>ds-protocol.c</t>
+  </si>
+  <si>
+    <t>ds-ipc-pal-socket.c</t>
+  </si>
+  <si>
+    <t>ds-dump-protocol.h</t>
+  </si>
+  <si>
+    <t>ds-eventpipe-protocol.h</t>
+  </si>
+  <si>
+    <t>ds-getter-setter.h</t>
+  </si>
+  <si>
+    <t>ds-ipc.h</t>
+  </si>
+  <si>
+    <t>ds-ipc-pal.h</t>
+  </si>
+  <si>
+    <t>ds-ipc-pal-types.h</t>
+  </si>
+  <si>
+    <t>ds-process-protocol.h</t>
+  </si>
+  <si>
+    <t>ds-profiler-protocol.h</t>
+  </si>
+  <si>
+    <t>ds-protocol.h</t>
+  </si>
+  <si>
+    <t>ds-rt.h</t>
+  </si>
+  <si>
+    <t>ds-rt-config.h</t>
+  </si>
+  <si>
+    <t>ds-rt-types.h</t>
+  </si>
+  <si>
+    <t>ds-server.h</t>
+  </si>
+  <si>
+    <t>ds-types.h</t>
+  </si>
+  <si>
+    <t>ds-ipc-pal-namedpipe.h</t>
+  </si>
+  <si>
+    <t>ds-ipc-pal-socket.h</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Pre-processor + header file ordering</t>
+  </si>
+  <si>
+    <t>Include this file in the EventSource files</t>
+  </si>
+  <si>
+    <t>Symbol not found</t>
+  </si>
+  <si>
+    <t>header file bringing in windows</t>
+  </si>
+  <si>
+    <t>try to isolate win defs</t>
+  </si>
+  <si>
+    <t>Issue#</t>
+  </si>
+  <si>
+    <t>Related_to</t>
+  </si>
+  <si>
+    <t>Issue_1</t>
+  </si>
+  <si>
+    <t>FreeLibrary</t>
+  </si>
+  <si>
+    <t>sample_profiler_unload_dependencies</t>
+  </si>
+  <si>
+    <t>obj file</t>
+  </si>
+  <si>
+    <t>ep-sources.c.obj</t>
+  </si>
+  <si>
+    <t>Issue_3</t>
+  </si>
+  <si>
+    <t>ds-sources.c.obj</t>
+  </si>
+  <si>
+    <t>24 more such symbols</t>
+  </si>
+  <si>
+    <t>19 for ds-sources.c.obj</t>
+  </si>
+  <si>
+    <t>6 for ep-sources.cobj</t>
+  </si>
+  <si>
+    <t>LoadLibraryW</t>
+  </si>
+  <si>
+    <t>sample_profiler_load_dependencies</t>
+  </si>
+  <si>
+    <t>Windows.h?</t>
+  </si>
+  <si>
+    <t>ep_rt_aot_walk_managed_stack_for_thread</t>
+  </si>
+  <si>
+    <t>ep_rt_walk_managed_stack_for_thread</t>
+  </si>
+  <si>
+    <t>EventPipeIpcStreamFactorySuspendedPortsCallback</t>
+  </si>
+  <si>
+    <t>ds_rt_port_array_alloc</t>
+  </si>
+  <si>
+    <t>ds_rt_port_array_is_valid</t>
+  </si>
+  <si>
+    <t>eventpipeadapter.h</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>ep_init</t>
+  </si>
+  <si>
+    <t>Callees</t>
+  </si>
+  <si>
+    <t>ep_requires_lock_not_held</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ep_rt_init</t>
+  </si>
+  <si>
+    <t>calls ep_rt_init in ep-rt-coreclr.h</t>
+  </si>
+  <si>
+    <t>runtime/ep-rt-coreclr.h at main · dotnet/runtime (github.com)</t>
+  </si>
+  <si>
+    <t>Inlined?</t>
+  </si>
+  <si>
+    <t>ep_thread_init</t>
+  </si>
+  <si>
+    <t>ep_rt_spin_lock_alloc</t>
+  </si>
+  <si>
+    <t>ep-rt-coreclr.h</t>
+  </si>
+  <si>
+    <t>ep_rt_thread_list_alloc</t>
+  </si>
+  <si>
+    <t>EP_RT_DEFINE_LIST (thread_list, ep_rt_thread_list_t, EventPipeThread *)</t>
+  </si>
+  <si>
+    <t>_rt_coreclr_list_alloc</t>
+  </si>
+  <si>
+    <t>ep_volatile_store_session</t>
+  </si>
+  <si>
+    <t>EP_MAX_NUMBER_OF_SESSIONS=64</t>
+  </si>
+  <si>
+    <t>ep_rt_volatile_store_ptr</t>
+  </si>
+  <si>
+    <t>Shim</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>ep_config_init</t>
+  </si>
+  <si>
+    <t>EP_RT_DEFINE_QUEUE (provider_callback_data_queue, ep_rt_provider_callback_data_queue_t, EventPipeProviderCallbackData *)</t>
+  </si>
+  <si>
+    <t>_rt_coreclr_queue_alloc (QUEUE_TYPE *queue)</t>
+  </si>
+  <si>
+    <t>ep_event_source_init</t>
+  </si>
+  <si>
+    <t>auto-generated code to initialize the runtime specific providers</t>
+  </si>
+  <si>
+    <t>and events so that the EventPipe configuration lock isn't taken at runtime</t>
+  </si>
+  <si>
+    <t>ep_sample_profiler_set_sampling_rate</t>
+  </si>
+  <si>
+    <t>sets to 1 msec</t>
+  </si>
+  <si>
+    <t>ep_rt_session_id_array_alloc</t>
+  </si>
+  <si>
+    <t>_ep_deferred_enable_session_ids</t>
+  </si>
+  <si>
+    <t>ep_rt_execution_checkpoint_array_alloc</t>
+  </si>
+  <si>
+    <t>ep_rt_volatile_store_uint32_t</t>
+  </si>
+  <si>
+    <t>EP_LOCK_ENTER (section1)</t>
+  </si>
+  <si>
+    <t>ep_volatile_store_eventpipe_state</t>
+  </si>
+  <si>
+    <t>EP_LOCK_EXIT (section1)</t>
+  </si>
+  <si>
+    <t>enable_default_session_via_env_variables</t>
+  </si>
+  <si>
+    <t>EventPipeAdapter::Initialize()</t>
+  </si>
+  <si>
+    <t>DiagnosticServerAdapter::Initialize()</t>
+  </si>
+  <si>
+    <t>DiagnosticServerAdapter::PauseForDiagnosticsMonitor()</t>
+  </si>
+  <si>
+    <t>EventPipeAdapter::FinishInitialize()</t>
+  </si>
+  <si>
+    <t>EventPipeAdapter::Shutdown()</t>
+  </si>
+  <si>
+    <t>DiagnosticServerAdapter::Shutdown()</t>
+  </si>
+  <si>
+    <t>EEStartupHelper</t>
+  </si>
+  <si>
+    <t>Init API Callee</t>
+  </si>
+  <si>
+    <t>Caller API</t>
+  </si>
+  <si>
+    <t>EEShutDownHelper</t>
+  </si>
+  <si>
+    <t>DS_RT_DEFINE_ARRAY (port_array, ds_rt_port_array_t, ds_rt_port_array_iterator_t, DiagnosticsPort *)</t>
+  </si>
+  <si>
+    <t>_rt_coreclr_array_alloc (ARRAY_TYPE *ep_array)</t>
+  </si>
+  <si>
+    <t>In ds-ipc.c</t>
+  </si>
+  <si>
+    <t>_rt_coreclr_array_is_valid (CONST_ARRAY_TYPE *ep_array)</t>
+  </si>
+  <si>
+    <t>ds_rt_config_value_get_enable</t>
+  </si>
+  <si>
+    <t>CLRConfig::GetConfigValue (CLRConfig::EXTERNAL_EnableDiagnostics) != 0;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1988,6 +2514,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF8250DF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2010,7 +2542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2040,6 +2572,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2056,6 +2589,121 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7B6C342A-E1A8-409B-B78E-8AA609D6C417}" name="Table2" displayName="Table2" ref="A1:A20" totalsRowShown="0">
+  <autoFilter ref="A1:A20" xr:uid="{7B6C342A-E1A8-409B-B78E-8AA609D6C417}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A20">
+    <sortCondition ref="A1:A20"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{413A0DC6-FE16-4E94-A0BF-16C61CA3F95E}" name="cmake"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E52BB174-8165-4044-8BDE-5A6BF7657A32}" name="Table3" displayName="Table3" ref="C1:C20" totalsRowShown="0">
+  <autoFilter ref="C1:C20" xr:uid="{E52BB174-8165-4044-8BDE-5A6BF7657A32}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:C20">
+    <sortCondition ref="C1:C20"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{114E07BD-033B-4914-AC14-4FBE83631787}" name="dir"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D46C85A2-C615-468E-B54F-C3351F01A293}" name="Table4" displayName="Table4" ref="E1:F10" totalsRowCount="1">
+  <autoFilter ref="E1:F9" xr:uid="{D46C85A2-C615-468E-B54F-C3351F01A293}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{94DFD56A-A3B7-4C33-BEB2-E5CDEA5F3577}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{E26708BD-FA69-4D39-A2FA-EAE356A73CD2}" name="Column2" totalsRowFunction="sum"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CE6C9B36-BFF3-4C86-A105-C3AF26B9373F}" name="Table5" displayName="Table5" ref="H1:H31" totalsRowShown="0">
+  <autoFilter ref="H1:H31" xr:uid="{CE6C9B36-BFF3-4C86-A105-C3AF26B9373F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:H31">
+    <sortCondition ref="H1:H31"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{8926C349-E07E-4B51-A84F-BC5FBF234E64}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BECAC722-F494-407B-8684-8CBAD49F023C}" name="Table6" displayName="Table6" ref="J1:J31" totalsRowShown="0">
+  <autoFilter ref="J1:J31" xr:uid="{BECAC722-F494-407B-8684-8CBAD49F023C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J2:J31">
+    <sortCondition ref="J1:J31"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{D9B993B9-7336-4106-A7E0-B5CE6FC4AF67}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A29829E5-6A03-474E-BA80-7F1462DC83C8}" name="Table7" displayName="Table7" ref="L1:L9" totalsRowShown="0">
+  <autoFilter ref="L1:L9" xr:uid="{A29829E5-6A03-474E-BA80-7F1462DC83C8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L2:L9">
+    <sortCondition ref="L1:L9"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{58E23A26-B8C2-4770-9B65-F5D112821E40}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EAE444FE-D1B3-400F-A2C0-41E382CFCDF2}" name="Table8" displayName="Table8" ref="N1:N11" totalsRowShown="0">
+  <autoFilter ref="N1:N11" xr:uid="{EAE444FE-D1B3-400F-A2C0-41E382CFCDF2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N2:N11">
+    <sortCondition ref="N1:N11"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{5934894E-3587-42E2-97DF-8CCA86CF04C8}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C7F37019-CA82-41F1-ACAE-AD32E7404A6C}" name="Table9" displayName="Table9" ref="P1:P15" totalsRowShown="0">
+  <autoFilter ref="P1:P15" xr:uid="{C7F37019-CA82-41F1-ACAE-AD32E7404A6C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P2:P15">
+    <sortCondition ref="P1:P15"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{E7245D18-1487-43AF-8C13-B765F4D0FCA5}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5FD1F61A-C7A8-4C90-9EA9-8FFED16F8A39}" name="Table10" displayName="Table10" ref="R1:R17" totalsRowShown="0">
+  <autoFilter ref="R1:R17" xr:uid="{5FD1F61A-C7A8-4C90-9EA9-8FFED16F8A39}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R2:R17">
+    <sortCondition ref="R1:R17"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{8E7A32F3-02EE-47DE-86E6-AB8F571A864B}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2469,13 +3117,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B10" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C10" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2541,6 +3189,180 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB36D2E8-A8B0-43B4-8B2A-10DC20F7FC67}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>539</v>
+      </c>
+      <c r="G1" t="s">
+        <v>423</v>
+      </c>
+      <c r="H1" t="s">
+        <v>427</v>
+      </c>
+      <c r="I1" t="s">
+        <v>425</v>
+      </c>
+      <c r="J1" t="s">
+        <v>426</v>
+      </c>
+      <c r="K1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>535</v>
+      </c>
+      <c r="C2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D2" t="s">
+        <v>534</v>
+      </c>
+      <c r="F2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G2" t="s">
+        <v>424</v>
+      </c>
+      <c r="H2" t="s">
+        <v>428</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="J2" t="s">
+        <v>331</v>
+      </c>
+      <c r="K2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>536</v>
+      </c>
+      <c r="C3" t="s">
+        <v>537</v>
+      </c>
+      <c r="D3" t="s">
+        <v>533</v>
+      </c>
+      <c r="F3" t="s">
+        <v>540</v>
+      </c>
+      <c r="G3" t="s">
+        <v>547</v>
+      </c>
+      <c r="H3" t="s">
+        <v>548</v>
+      </c>
+      <c r="I3" t="s">
+        <v>549</v>
+      </c>
+      <c r="K3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>535</v>
+      </c>
+      <c r="F4" t="s">
+        <v>545</v>
+      </c>
+      <c r="G4" t="s">
+        <v>541</v>
+      </c>
+      <c r="H4" t="s">
+        <v>552</v>
+      </c>
+      <c r="I4" t="s">
+        <v>542</v>
+      </c>
+      <c r="J4" t="s">
+        <v>441</v>
+      </c>
+      <c r="K4" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>545</v>
+      </c>
+      <c r="G5" t="s">
+        <v>550</v>
+      </c>
+      <c r="H5" t="s">
+        <v>552</v>
+      </c>
+      <c r="I5" t="s">
+        <v>551</v>
+      </c>
+      <c r="K5" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>545</v>
+      </c>
+      <c r="G6" t="s">
+        <v>553</v>
+      </c>
+      <c r="I6" t="s">
+        <v>554</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D2F1AD-2A04-472D-8139-884175DD7E01}">
   <dimension ref="A1:F23"/>
   <sheetViews>
@@ -2559,182 +3381,182 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="B1" t="s">
         <v>135</v>
       </c>
       <c r="D1" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="E1" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="F1" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="D2" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="F4" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="B5" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="D5" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="D6" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="B8" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="D8" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="E8" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="D9" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="B11" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="D12" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="D13" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="B15" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="D16" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="E16" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="D17" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="B19" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="D19" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="B21" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="B23" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -2743,148 +3565,936 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5CE37D-047E-48E6-B103-516D9C44DD99}">
-  <dimension ref="A1:D3"/>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B29259E-9E3E-4368-A627-329A1EE53041}">
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="119.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>602</v>
       </c>
       <c r="B1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>340</v>
-      </c>
       <c r="D1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="E1" t="s">
+        <v>561</v>
+      </c>
+      <c r="F1" t="s">
+        <v>563</v>
+      </c>
+      <c r="G1" t="s">
+        <v>577</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>345</v>
+        <v>595</v>
       </c>
       <c r="B2" t="s">
-        <v>344</v>
+        <v>601</v>
       </c>
       <c r="C2" t="s">
-        <v>341</v>
+        <v>558</v>
       </c>
       <c r="D2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>345</v>
-      </c>
-      <c r="B3" t="s">
-        <v>346</v>
-      </c>
-      <c r="D3" t="s">
-        <v>347</v>
+        <v>560</v>
+      </c>
+      <c r="E2" t="s">
+        <v>562</v>
+      </c>
+      <c r="F2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>564</v>
+      </c>
+      <c r="F3" t="s">
+        <v>565</v>
+      </c>
+      <c r="G3" t="s">
+        <v>578</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>568</v>
+      </c>
+      <c r="F4" t="s">
+        <v>569</v>
+      </c>
+      <c r="G4" t="s">
+        <v>578</v>
+      </c>
+      <c r="H4" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>571</v>
+      </c>
+      <c r="G5" t="s">
+        <v>578</v>
+      </c>
+      <c r="H5" t="s">
+        <v>572</v>
+      </c>
+      <c r="I5" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>574</v>
+      </c>
+      <c r="F6" t="s">
+        <v>576</v>
+      </c>
+      <c r="G6" t="s">
+        <v>578</v>
+      </c>
+      <c r="H6" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>579</v>
+      </c>
+      <c r="F7" t="s">
+        <v>581</v>
+      </c>
+      <c r="G7" t="s">
+        <v>578</v>
+      </c>
+      <c r="H7" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>435</v>
+      </c>
+      <c r="E8" t="s">
+        <v>582</v>
+      </c>
+      <c r="F8" t="s">
+        <v>583</v>
+      </c>
+      <c r="H8" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>585</v>
+      </c>
+      <c r="F9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>587</v>
+      </c>
+      <c r="F10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G10" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>587</v>
+      </c>
+      <c r="F11" t="s">
+        <v>587</v>
+      </c>
+      <c r="G11" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>589</v>
+      </c>
+      <c r="G12" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>592</v>
+      </c>
+      <c r="F14" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>596</v>
+      </c>
+      <c r="B18" t="s">
+        <v>601</v>
+      </c>
+      <c r="C18" t="s">
+        <v>331</v>
+      </c>
+      <c r="D18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>333</v>
+      </c>
+      <c r="F19" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>555</v>
+      </c>
+      <c r="H20" t="s">
+        <v>605</v>
+      </c>
+      <c r="I20" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>556</v>
+      </c>
+      <c r="H21" t="s">
+        <v>605</v>
+      </c>
+      <c r="I21" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>609</v>
+      </c>
+      <c r="H23" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>597</v>
+      </c>
+      <c r="B36" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>598</v>
+      </c>
+      <c r="B38" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>599</v>
+      </c>
+      <c r="B40" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>600</v>
+      </c>
+      <c r="B42" t="s">
+        <v>604</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" location="L1299" display="https://github.com/dotnet/runtime/blob/main/src/coreclr/vm/eventing/eventpipe/ep-rt-coreclr.h - L1299" xr:uid="{81143E76-694D-4869-BFE8-060FB84A0140}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E79789-F7A8-4F49-8B82-CFB73A3CAE8C}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" t="s">
-        <v>135</v>
+        <v>477</v>
       </c>
       <c r="C1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>478</v>
+      </c>
+      <c r="E1" t="s">
+        <v>467</v>
+      </c>
+      <c r="F1" t="s">
+        <v>468</v>
+      </c>
+      <c r="H1" t="s">
+        <v>467</v>
+      </c>
+      <c r="J1" t="s">
+        <v>467</v>
+      </c>
+      <c r="L1" t="s">
+        <v>467</v>
+      </c>
+      <c r="N1" t="s">
+        <v>467</v>
+      </c>
+      <c r="P1" t="s">
+        <v>467</v>
+      </c>
+      <c r="R1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" t="s">
-        <v>126</v>
+        <v>429</v>
       </c>
       <c r="C2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+      <c r="E2" t="s">
+        <v>469</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>479</v>
+      </c>
+      <c r="J2" t="s">
+        <v>479</v>
+      </c>
+      <c r="L2" t="s">
+        <v>510</v>
+      </c>
+      <c r="N2" t="s">
+        <v>510</v>
+      </c>
+      <c r="P2" t="s">
+        <v>516</v>
+      </c>
+      <c r="R2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" t="s">
-        <v>126</v>
+        <v>431</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+      <c r="E3" t="s">
+        <v>470</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>480</v>
+      </c>
+      <c r="J3" t="s">
+        <v>480</v>
+      </c>
+      <c r="L3" t="s">
+        <v>511</v>
+      </c>
+      <c r="N3" t="s">
+        <v>511</v>
+      </c>
+      <c r="P3" t="s">
+        <v>517</v>
+      </c>
+      <c r="R3" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+      <c r="C4" t="s">
+        <v>451</v>
+      </c>
+      <c r="E4" t="s">
+        <v>471</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>481</v>
+      </c>
+      <c r="J4" t="s">
+        <v>481</v>
+      </c>
+      <c r="L4" t="s">
+        <v>332</v>
+      </c>
+      <c r="N4" t="s">
+        <v>332</v>
+      </c>
+      <c r="P4" t="s">
+        <v>518</v>
+      </c>
+      <c r="R4" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C5" t="s">
+        <v>452</v>
+      </c>
+      <c r="E5" t="s">
+        <v>472</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>482</v>
+      </c>
+      <c r="J5" t="s">
+        <v>482</v>
+      </c>
+      <c r="L5" t="s">
+        <v>512</v>
+      </c>
+      <c r="N5" t="s">
+        <v>428</v>
+      </c>
+      <c r="P5" t="s">
+        <v>519</v>
+      </c>
+      <c r="R5" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" t="s">
-        <v>131</v>
+        <v>436</v>
+      </c>
+      <c r="C6" t="s">
+        <v>453</v>
+      </c>
+      <c r="E6" t="s">
+        <v>476</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>483</v>
+      </c>
+      <c r="J6" t="s">
+        <v>483</v>
+      </c>
+      <c r="L6" t="s">
+        <v>513</v>
+      </c>
+      <c r="N6" t="s">
+        <v>515</v>
+      </c>
+      <c r="P6" t="s">
+        <v>520</v>
+      </c>
+      <c r="R6" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>433</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>454</v>
+      </c>
+      <c r="E7" t="s">
+        <v>473</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>484</v>
+      </c>
+      <c r="J7" t="s">
+        <v>484</v>
+      </c>
+      <c r="L7" t="s">
+        <v>514</v>
+      </c>
+      <c r="N7" t="s">
+        <v>512</v>
+      </c>
+      <c r="P7" t="s">
+        <v>521</v>
+      </c>
+      <c r="R7" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>434</v>
+      </c>
+      <c r="C8" t="s">
+        <v>455</v>
+      </c>
+      <c r="E8" t="s">
+        <v>474</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>485</v>
+      </c>
+      <c r="J8" t="s">
+        <v>485</v>
+      </c>
+      <c r="L8" t="s">
+        <v>331</v>
+      </c>
+      <c r="N8" t="s">
+        <v>513</v>
+      </c>
+      <c r="P8" t="s">
+        <v>522</v>
+      </c>
+      <c r="R8" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>435</v>
+      </c>
+      <c r="C9" t="s">
+        <v>456</v>
+      </c>
+      <c r="E9" t="s">
+        <v>475</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>486</v>
+      </c>
+      <c r="J9" t="s">
+        <v>486</v>
+      </c>
+      <c r="L9" t="s">
+        <v>509</v>
+      </c>
+      <c r="N9" t="s">
+        <v>514</v>
+      </c>
+      <c r="P9" t="s">
+        <v>523</v>
+      </c>
+      <c r="R9" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>437</v>
+      </c>
+      <c r="C10" t="s">
+        <v>457</v>
+      </c>
+      <c r="F10">
+        <f>SUBTOTAL(109,Table4[Column2])</f>
+        <v>80</v>
+      </c>
+      <c r="H10" t="s">
+        <v>487</v>
+      </c>
+      <c r="J10" t="s">
+        <v>487</v>
+      </c>
+      <c r="N10" t="s">
+        <v>331</v>
+      </c>
+      <c r="P10" t="s">
+        <v>524</v>
+      </c>
+      <c r="R10" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>438</v>
+      </c>
+      <c r="C11" t="s">
+        <v>458</v>
+      </c>
+      <c r="H11" t="s">
+        <v>488</v>
+      </c>
+      <c r="J11" t="s">
+        <v>488</v>
+      </c>
+      <c r="N11" t="s">
+        <v>509</v>
+      </c>
+      <c r="P11" t="s">
+        <v>525</v>
+      </c>
+      <c r="R11" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>439</v>
+      </c>
+      <c r="C12" t="s">
+        <v>459</v>
+      </c>
+      <c r="H12" t="s">
+        <v>489</v>
+      </c>
+      <c r="J12" t="s">
+        <v>489</v>
+      </c>
+      <c r="P12" t="s">
+        <v>526</v>
+      </c>
+      <c r="R12" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>440</v>
+      </c>
+      <c r="C13" t="s">
+        <v>460</v>
+      </c>
+      <c r="H13" t="s">
+        <v>490</v>
+      </c>
+      <c r="J13" t="s">
+        <v>490</v>
+      </c>
+      <c r="P13" t="s">
+        <v>527</v>
+      </c>
+      <c r="R13" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>441</v>
+      </c>
+      <c r="C14" t="s">
+        <v>461</v>
+      </c>
+      <c r="H14" t="s">
+        <v>491</v>
+      </c>
+      <c r="J14" t="s">
+        <v>491</v>
+      </c>
+      <c r="P14" t="s">
+        <v>528</v>
+      </c>
+      <c r="R14" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>443</v>
+      </c>
+      <c r="C15" t="s">
+        <v>462</v>
+      </c>
+      <c r="H15" t="s">
+        <v>492</v>
+      </c>
+      <c r="J15" t="s">
+        <v>492</v>
+      </c>
+      <c r="P15" t="s">
+        <v>529</v>
+      </c>
+      <c r="R15" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>442</v>
+      </c>
+      <c r="C16" t="s">
+        <v>463</v>
+      </c>
+      <c r="H16" t="s">
+        <v>493</v>
+      </c>
+      <c r="J16" t="s">
+        <v>493</v>
+      </c>
+      <c r="R16" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>444</v>
+      </c>
+      <c r="C17" t="s">
+        <v>448</v>
+      </c>
+      <c r="H17" t="s">
+        <v>494</v>
+      </c>
+      <c r="J17" t="s">
+        <v>494</v>
+      </c>
+      <c r="R17" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>445</v>
+      </c>
+      <c r="C18" t="s">
+        <v>464</v>
+      </c>
+      <c r="H18" t="s">
+        <v>495</v>
+      </c>
+      <c r="J18" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>446</v>
+      </c>
+      <c r="C19" t="s">
+        <v>465</v>
+      </c>
+      <c r="H19" t="s">
+        <v>496</v>
+      </c>
+      <c r="J19" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>447</v>
+      </c>
+      <c r="C20" t="s">
+        <v>466</v>
+      </c>
+      <c r="H20" t="s">
+        <v>497</v>
+      </c>
+      <c r="J20" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>498</v>
+      </c>
+      <c r="J21" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>499</v>
+      </c>
+      <c r="J22" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>500</v>
+      </c>
+      <c r="J23" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>501</v>
+      </c>
+      <c r="J24" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>502</v>
+      </c>
+      <c r="J25" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>503</v>
+      </c>
+      <c r="J26" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>504</v>
+      </c>
+      <c r="J27" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>505</v>
+      </c>
+      <c r="J28" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>506</v>
+      </c>
+      <c r="J29" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>507</v>
+      </c>
+      <c r="J30" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>508</v>
+      </c>
+      <c r="J31" t="s">
+        <v>508</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="9">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2971,10 +4581,10 @@
         <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="F4" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3033,7 +4643,7 @@
         <v>84</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3124,7 +4734,7 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D16" t="s">
         <v>28</v>
@@ -3184,71 +4794,71 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B22" t="s">
         <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B23" t="s">
         <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
         <v>84</v>
       </c>
       <c r="C24" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B25" t="s">
         <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D25" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B26" t="s">
         <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C27" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D27" t="s">
         <v>126</v>
@@ -3256,13 +4866,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
@@ -3270,13 +4880,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D29" t="s">
         <v>28</v>
@@ -3284,13 +4894,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B30" t="s">
         <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3442,7 +5052,7 @@
         <v>114</v>
       </c>
       <c r="C13" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3530,7 +5140,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3538,103 +5148,103 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B11" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B12" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B13" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B14" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3663,84 +5273,84 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" t="s">
         <v>193</v>
-      </c>
-      <c r="B4" t="s">
-        <v>195</v>
-      </c>
-      <c r="C4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D4" t="s">
-        <v>195</v>
-      </c>
-      <c r="E4" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" t="s">
         <v>195</v>
       </c>
-      <c r="D5" t="s">
-        <v>204</v>
-      </c>
       <c r="E5" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="E6" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="F6" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3756,7 +5366,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3769,95 +5379,95 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
         <v>135</v>
       </c>
       <c r="C1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="D1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" t="s">
         <v>214</v>
       </c>
-      <c r="B2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D2" t="s">
-        <v>224</v>
-      </c>
       <c r="F2" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C3" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="D3" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="F3" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="F4" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C5" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C6" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D6" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -3882,10 +5492,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3893,69 +5503,69 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B5" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B9" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C9" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3966,10 +5576,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA29BBC-4F7B-49AE-9AF5-58895851EE5E}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3982,237 +5592,237 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="F1" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="B2" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C2" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="D2" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="E2" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B3" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C3" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="D3" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="E3" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B4" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C4" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D4" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="E4" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B5" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C5" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="D5" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B6" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="C6" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="D6" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="E6" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="C7" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="E7" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="D8" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="E8" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B9" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C9" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D9" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="E9" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B10" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="C10" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="D10" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="E10" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="C11" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="D11" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="E11" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B12" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="C12" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D12" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B13" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="C13" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D13" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B14" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="C14" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D14" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="E14" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="F14">
         <v>500</v>
@@ -4220,167 +5830,175 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B15" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="C15" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D15" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="E15" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>287</v>
+      </c>
+      <c r="B16" t="s">
+        <v>315</v>
+      </c>
+      <c r="C16" t="s">
+        <v>284</v>
+      </c>
+      <c r="D16" t="s">
         <v>297</v>
       </c>
-      <c r="B16" t="s">
-        <v>325</v>
-      </c>
-      <c r="C16" t="s">
-        <v>294</v>
-      </c>
-      <c r="D16" t="s">
-        <v>307</v>
-      </c>
       <c r="E16" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="F16" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B17" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="C17" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D17" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="E17" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="F17" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B18" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="C18" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="D18" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="B19" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="C19" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="D19" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="B20" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="C20" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="D20" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="E20" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="B21" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="C21" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="D21" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="B22" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="C22" t="s">
+        <v>401</v>
+      </c>
+      <c r="D22" t="s">
         <v>415</v>
       </c>
-      <c r="D22" t="s">
-        <v>429</v>
-      </c>
       <c r="E22" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
       <c r="B23" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="C23" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="E23" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="F23" t="s">
-        <v>435</v>
+        <v>421</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="13" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F26" r:id="rId1" xr:uid="{0C6A3BB0-8821-4BC1-BCC3-B8D8224FE366}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4402,19 +6020,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="B1" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="C1" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="D1" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="E1" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -4422,16 +6040,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="D2" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="E2" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="F2" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4439,52 +6057,52 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="D3" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="E3" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="F3" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="D4" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="E4" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="F4" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="D5" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="E5" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="D6" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="E6" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4492,10 +6110,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="D7" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4503,16 +6121,16 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="C8" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="D8" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="E8" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4520,91 +6138,91 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="C9" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="D9" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="E9" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="10" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="26" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="27" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="28" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
     </row>
     <row r="29" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
     </row>
     <row r="30" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="31" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="32" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
     </row>
     <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
     </row>
     <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
     </row>
     <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
     </row>
     <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
post compiler notes and state
</commit_message>
<xml_diff>
--- a/src/aot/NativeAOT.xlsx
+++ b/src/aot/NativeAOT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Core\LakshanF\CSharp\src\aot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4BE3B4-859C-4C31-B204-8F0E9213D2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7926CA-D25C-4141-B15F-70EA7658238A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="12" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="11" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="SDK" sheetId="4" r:id="rId1"/>
@@ -25,9 +25,11 @@
     <sheet name="Port-Issues-linker" sheetId="13" r:id="rId10"/>
     <sheet name="Port-Tables" sheetId="12" r:id="rId11"/>
     <sheet name="EP_Init" sheetId="14" r:id="rId12"/>
-    <sheet name="scratch" sheetId="5" r:id="rId13"/>
+    <sheet name="EventSource sources" sheetId="5" r:id="rId13"/>
+    <sheet name="scratch" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="636">
   <si>
     <t>File</t>
   </si>
@@ -2270,9 +2272,6 @@
     <t>runtime/ep-rt-coreclr.h at main · dotnet/runtime (github.com)</t>
   </si>
   <si>
-    <t>Inlined?</t>
-  </si>
-  <si>
     <t>ep_thread_init</t>
   </si>
   <si>
@@ -2288,9 +2287,6 @@
     <t>EP_RT_DEFINE_LIST (thread_list, ep_rt_thread_list_t, EventPipeThread *)</t>
   </si>
   <si>
-    <t>_rt_coreclr_list_alloc</t>
-  </si>
-  <si>
     <t>ep_volatile_store_session</t>
   </si>
   <si>
@@ -2400,6 +2396,87 @@
   </si>
   <si>
     <t>CLRConfig::GetConfigValue (CLRConfig::EXTERNAL_EnableDiagnostics) != 0;</t>
+  </si>
+  <si>
+    <t>ds_ipc_pal_init</t>
+  </si>
+  <si>
+    <t>Initialize PAL layer.</t>
+  </si>
+  <si>
+    <t>ds_ipc_advertise_cookie_v1_init</t>
+  </si>
+  <si>
+    <t>Initialize the RuntimeIndentifier before use</t>
+  </si>
+  <si>
+    <t>@TODO - not called</t>
+  </si>
+  <si>
+    <t>ds_ipc_stream_factory_configure</t>
+  </si>
+  <si>
+    <t>ds_ipc_stream_factory_any_suspended_ports</t>
+  </si>
+  <si>
+    <t>ds_ipc_stream_factory_has_active_ports</t>
+  </si>
+  <si>
+    <t>ep_volatile_load_eventpipe_state</t>
+  </si>
+  <si>
+    <t>check not already initialized</t>
+  </si>
+  <si>
+    <t>!= EP_STATE_NOT_INITIALIZED</t>
+  </si>
+  <si>
+    <t>Initialize critical section,  get CLRConfig::INTERNAL_EventPipeProcNumbers, setup the windows processor group offset table</t>
+  </si>
+  <si>
+    <t>allocate thread lock (initializes spin lock - spin_lock-&gt;lock-&gt;Init (LOCK_TYPE_DEFAULT))</t>
+  </si>
+  <si>
+    <t>_rt_coreclr_list_alloc - allocate thread lists (to keep the threads?)</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t>commandData</t>
+  </si>
+  <si>
+    <t>new byte[5]</t>
+  </si>
+  <si>
+    <t>buf[0]==1</t>
+  </si>
+  <si>
+    <t>MaxShortPayload</t>
+  </si>
+  <si>
+    <t>buf</t>
+  </si>
+  <si>
+    <t>payload</t>
+  </si>
+  <si>
+    <t>Encode (num bytes)</t>
+  </si>
+  <si>
+    <t>Decode (num bytes)</t>
+  </si>
+  <si>
+    <t>MaxRawShortPayload</t>
+  </si>
+  <si>
+    <t>DehydratedDataCommandPayloadShift</t>
+  </si>
+  <si>
+    <t>Inlined? More like checked (EP_CHECKED_BUILD)</t>
+  </si>
+  <si>
+    <t>ep.c implementation calls ep_rt_config_requires_lock_held, which calls ep_rt_lock_requires_lock_held(ep_rt_coreclr_config_lock_get ())</t>
   </si>
 </sst>
 </file>
@@ -3567,10 +3644,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B29259E-9E3E-4368-A627-329A1EE53041}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3579,19 +3656,19 @@
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="58.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="119.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="54" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="116.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -3606,7 +3683,7 @@
         <v>563</v>
       </c>
       <c r="G1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -3617,10 +3694,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C2" t="s">
         <v>558</v>
@@ -3632,7 +3709,10 @@
         <v>562</v>
       </c>
       <c r="F2" t="s">
-        <v>567</v>
+        <v>634</v>
+      </c>
+      <c r="H2" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3643,182 +3723,188 @@
         <v>565</v>
       </c>
       <c r="G3" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>566</v>
       </c>
+      <c r="I3" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
+        <v>617</v>
+      </c>
+      <c r="F4" t="s">
+        <v>618</v>
+      </c>
+      <c r="H4" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>567</v>
+      </c>
+      <c r="F5" t="s">
         <v>568</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G5" t="s">
+        <v>576</v>
+      </c>
+      <c r="H5" t="s">
         <v>569</v>
       </c>
-      <c r="G4" t="s">
-        <v>578</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I5" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
+      <c r="G6" t="s">
+        <v>576</v>
+      </c>
+      <c r="H6" t="s">
         <v>571</v>
       </c>
-      <c r="G5" t="s">
-        <v>578</v>
-      </c>
-      <c r="H5" t="s">
-        <v>572</v>
-      </c>
-      <c r="I5" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>574</v>
-      </c>
-      <c r="F6" t="s">
-        <v>576</v>
-      </c>
-      <c r="G6" t="s">
-        <v>578</v>
-      </c>
-      <c r="H6" t="s">
-        <v>575</v>
+      <c r="I6" t="s">
+        <v>622</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
+        <v>572</v>
+      </c>
+      <c r="F7" t="s">
+        <v>574</v>
+      </c>
+      <c r="G7" t="s">
+        <v>576</v>
+      </c>
+      <c r="H7" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>577</v>
+      </c>
+      <c r="F8" t="s">
         <v>579</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G8" t="s">
+        <v>576</v>
+      </c>
+      <c r="H8" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>435</v>
+      </c>
+      <c r="E9" t="s">
+        <v>580</v>
+      </c>
+      <c r="F9" t="s">
         <v>581</v>
       </c>
-      <c r="G7" t="s">
-        <v>578</v>
-      </c>
-      <c r="H7" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>435</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="H9" t="s">
         <v>582</v>
-      </c>
-      <c r="F8" t="s">
-        <v>583</v>
-      </c>
-      <c r="H8" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>585</v>
-      </c>
-      <c r="F9" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="F10" t="s">
-        <v>588</v>
-      </c>
-      <c r="G10" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F11" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G11" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>589</v>
+        <v>585</v>
+      </c>
+      <c r="F12" t="s">
+        <v>585</v>
       </c>
       <c r="G12" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>591</v>
+        <v>587</v>
+      </c>
+      <c r="G13" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>592</v>
-      </c>
-      <c r="F14" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>593</v>
+        <v>590</v>
+      </c>
+      <c r="F15" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>596</v>
-      </c>
-      <c r="B18" t="s">
-        <v>601</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B19" t="s">
+        <v>599</v>
+      </c>
+      <c r="C19" t="s">
         <v>331</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
         <v>333</v>
       </c>
-      <c r="F19" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>555</v>
-      </c>
-      <c r="H20" t="s">
         <v>605</v>
-      </c>
-      <c r="I20" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="H21" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="I21" t="s">
         <v>606</v>
@@ -3826,47 +3912,92 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
+        <v>556</v>
+      </c>
+      <c r="H22" t="s">
+        <v>603</v>
+      </c>
+      <c r="I22" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>607</v>
+      </c>
+      <c r="H24" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
         <v>609</v>
       </c>
-      <c r="H23" t="s">
+      <c r="F25" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="H25" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>611</v>
+      </c>
+      <c r="F26" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>595</v>
+      </c>
+      <c r="B37" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>596</v>
+      </c>
+      <c r="B39" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>597</v>
       </c>
-      <c r="B36" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B41" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>598</v>
       </c>
-      <c r="B38" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>599</v>
-      </c>
-      <c r="B40" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>600</v>
-      </c>
-      <c r="B42" t="s">
-        <v>604</v>
+      <c r="B43" t="s">
+        <v>602</v>
       </c>
     </row>
   </sheetData>
@@ -3881,7 +4012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E79789-F7A8-4F49-8B82-CFB73A3CAE8C}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -4495,6 +4626,95 @@
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40389D47-332F-4BA8-AEE5-76C6B7E667AC}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B1">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>623</v>
+      </c>
+      <c r="E1" t="s">
+        <v>624</v>
+      </c>
+      <c r="F1" t="s">
+        <v>628</v>
+      </c>
+      <c r="H1" t="s">
+        <v>630</v>
+      </c>
+      <c r="J1" t="s">
+        <v>631</v>
+      </c>
+      <c r="K1" t="s">
+        <v>623</v>
+      </c>
+      <c r="L1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2">
+        <v>63</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>625</v>
+      </c>
+      <c r="H2" t="s">
+        <v>626</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>633</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5578,8 +5798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA29BBC-4F7B-49AE-9AF5-58895851EE5E}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6006,7 +6226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8B967F-830C-4BFE-AD9E-62679C946E39}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating trace client to build under runtime repo
</commit_message>
<xml_diff>
--- a/src/aot/NativeAOT.xlsx
+++ b/src/aot/NativeAOT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Core\LakshanF\CSharp\src\aot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7926CA-D25C-4141-B15F-70EA7658238A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CA8041F-58F0-454F-8FC9-0204FE76CB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="11" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
   </bookViews>
@@ -3647,7 +3647,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
standalong diag ep test
</commit_message>
<xml_diff>
--- a/src/aot/NativeAOT.xlsx
+++ b/src/aot/NativeAOT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Core\LakshanF\CSharp\src\aot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\core\LakshanF\CSharp\src\aot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CA8041F-58F0-454F-8FC9-0204FE76CB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C1DE77-9D96-4DB8-9909-C158BAF79969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="11" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="SDK" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <sheet name="scratch" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="645">
   <si>
     <t>File</t>
   </si>
@@ -2477,6 +2476,33 @@
   </si>
   <si>
     <t>ep.c implementation calls ep_rt_config_requires_lock_held, which calls ep_rt_lock_requires_lock_held(ep_rt_coreclr_config_lock_get ())</t>
+  </si>
+  <si>
+    <t>13.5 M</t>
+  </si>
+  <si>
+    <t>12 M</t>
+  </si>
+  <si>
+    <t>EP - bin\coreclr\windows.x64.Debug\aotsdk</t>
+  </si>
+  <si>
+    <t>Main - bin\coreclr\windows.x64.Debug\aotsdk</t>
+  </si>
+  <si>
+    <t>8.9 M</t>
+  </si>
+  <si>
+    <t>11.7 M</t>
+  </si>
+  <si>
+    <t>C:\work\core\CurrentWork\runtime\src\coreclr\tools\aot\ILCompiler\reproNative\x64\Debug\reproNative.exe</t>
+  </si>
+  <si>
+    <t>Both managed and native off</t>
+  </si>
+  <si>
+    <t>7.6M</t>
   </si>
 </sst>
 </file>
@@ -3646,7 +3672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B29259E-9E3E-4368-A627-329A1EE53041}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -5583,10 +5609,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A474016-A235-45A8-AC3E-8B82CE76D8C1}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5594,10 +5620,15 @@
     <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="76.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="103.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>203</v>
       </c>
@@ -5610,8 +5641,23 @@
       <c r="D1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>639</v>
+      </c>
+      <c r="I1" t="s">
+        <v>638</v>
+      </c>
+      <c r="K1" t="s">
+        <v>643</v>
+      </c>
+      <c r="L1" t="s">
+        <v>644</v>
+      </c>
+      <c r="M1" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -5627,8 +5673,14 @@
       <c r="F2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>640</v>
+      </c>
+      <c r="I2" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>207</v>
       </c>
@@ -5644,8 +5696,14 @@
       <c r="F3" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>641</v>
+      </c>
+      <c r="I3" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>209</v>
       </c>
@@ -5661,8 +5719,14 @@
       <c r="F4" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>641</v>
+      </c>
+      <c r="I4" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>220</v>
       </c>
@@ -5676,7 +5740,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>221</v>
       </c>

</xml_diff>

<commit_message>
partially fixed NativeAOT repro
</commit_message>
<xml_diff>
--- a/src/aot/NativeAOT.xlsx
+++ b/src/aot/NativeAOT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\core\LakshanF\CSharp\src\aot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C1DE77-9D96-4DB8-9909-C158BAF79969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7109D96E-BC9E-4B28-ACD7-D5E202D18E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
+    <workbookView xWindow="38280" yWindow="1755" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="14" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="SDK" sheetId="4" r:id="rId1"/>
@@ -26,9 +26,12 @@
     <sheet name="Port-Tables" sheetId="12" r:id="rId11"/>
     <sheet name="EP_Init" sheetId="14" r:id="rId12"/>
     <sheet name="EventSource sources" sheetId="5" r:id="rId13"/>
-    <sheet name="scratch" sheetId="15" r:id="rId14"/>
+    <sheet name="HeaderFiles" sheetId="16" r:id="rId14"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId15"/>
+    <sheet name="scratch" sheetId="15" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="656">
   <si>
     <t>File</t>
   </si>
@@ -2503,6 +2506,39 @@
   </si>
   <si>
     <t>7.6M</t>
+  </si>
+  <si>
+    <t>ep-rt-aot.cpp</t>
+  </si>
+  <si>
+    <t>#include "gcenv.h"</t>
+  </si>
+  <si>
+    <t>#include "regdisplay.h"</t>
+  </si>
+  <si>
+    <t>#include "StackFrameIterator.h"</t>
+  </si>
+  <si>
+    <t>#include "thread.h"</t>
+  </si>
+  <si>
+    <t>#include "holder.h"</t>
+  </si>
+  <si>
+    <t>#include "SpinLock.h"</t>
+  </si>
+  <si>
+    <t>ep-rt-aot.h</t>
+  </si>
+  <si>
+    <t>#ifdef _INC_WINDOWS</t>
+  </si>
+  <si>
+    <t>#include &lt;sysinfoapi.h&gt;</t>
+  </si>
+  <si>
+    <t>#endif</t>
   </si>
 </sst>
 </file>
@@ -4656,6 +4692,108 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2557EFB-44BC-4596-B2FD-75E3B0B9E645}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B1" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>646</v>
+      </c>
+      <c r="B2" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>647</v>
+      </c>
+      <c r="B3" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>648</v>
+      </c>
+      <c r="B4" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>649</v>
+      </c>
+      <c r="B5" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>650</v>
+      </c>
+      <c r="B6" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>651</v>
+      </c>
+      <c r="B7" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>655</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC765001-6D80-4D34-8B75-741B58122490}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40389D47-332F-4BA8-AEE5-76C6B7E667AC}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -5611,7 +5749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A474016-A235-45A8-AC3E-8B82CE76D8C1}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update for implicit pks reference
</commit_message>
<xml_diff>
--- a/src/aot/NativeAOT.xlsx
+++ b/src/aot/NativeAOT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\core\LakshanF\CSharp\src\aot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7109D96E-BC9E-4B28-ACD7-D5E202D18E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7FB9C4-5DE7-4E2F-93A4-6B94EF8D0C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1755" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="14" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{566134FB-1CD2-4FEE-B945-728C01B79D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="SDK" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <sheet name="scratch" sheetId="15" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="671">
   <si>
     <t>File</t>
   </si>
@@ -2539,6 +2538,246 @@
   </si>
   <si>
     <t>#endif</t>
+  </si>
+  <si>
+    <t>.NET 8</t>
+  </si>
+  <si>
+    <t>eventpipe-disabled.lib</t>
+  </si>
+  <si>
+    <t>C:\Users\lakshanf\.nuget\packages\runtime.win-x64.microsoft.dotnet.ilcompiler\8.0.0-preview.2.23128.3\sdk\eventpipe-disabled.lib</t>
+  </si>
+  <si>
+    <t>Net 8.0</t>
+  </si>
+  <si>
+    <t>Microsoft.DotNet.ILCompiler.props</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ILCompilerTargetsPath</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF24292F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;$(MSBuildThisFileDirectory)Microsoft.DotNet.ILCompiler.SingleEntry.targets&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ILCompilerTargetsPath</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF24292F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Implicit package Reference imports the package</t>
+  </si>
+  <si>
+    <t>No Microsoft.DotNet.ILCompiler import from Microsoft.NET.Sdk.props</t>
+  </si>
+  <si>
+    <t>Nuget Restore: Ilcompiler package is downloaded isntead of relying on SDK</t>
+  </si>
+  <si>
+    <t>SDK does not have a stale copy of the build targets, instead runtime pack version is the default</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Import</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"$(ILCompilerTargetsPath)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Condition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"'$(ILCompilerTargetsPath)' != '' and '$(PublishAot)' == 'true'"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>dotnet\sdk\8.0.100-preview.2.23157.25\Sdks\Microsoft.NET.Sdk\targets\Microsoft.NET.Sdk.targets</t>
+  </si>
+  <si>
+    <t>If the user has explicit package reference (discouraged)</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Import</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"$(MSBuildThisFileDirectory)\Microsoft.NETCore.Native.targets"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF808080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>/&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Now ok</t>
   </si>
 </sst>
 </file>
@@ -3142,10 +3381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BA1F5E-206C-47BA-9ABB-2AD1328C0FAB}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3322,8 +3561,62 @@
         <v>47</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>662</v>
+      </c>
+      <c r="B20" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>664</v>
+      </c>
+      <c r="B21" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="B22" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="B23" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="B25" t="s">
+        <v>670</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4785,7 +5078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC765001-6D80-4D34-8B75-741B58122490}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -4887,7 +5180,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5495,10 +5788,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F2192D-3A65-4BCE-88B7-89B17384964D}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5629,6 +5922,17 @@
       </c>
       <c r="B15" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>656</v>
+      </c>
+      <c r="B18" t="s">
+        <v>657</v>
+      </c>
+      <c r="C18" t="s">
+        <v>658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>